<commit_message>
data is taken from Excel
</commit_message>
<xml_diff>
--- a/src/TestData/Data.xlsx
+++ b/src/TestData/Data.xlsx
@@ -4,13 +4,14 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14835" windowHeight="6075" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
     <sheet name="Leads" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A2:N19"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="15">
   <si>
     <t>TCName</t>
   </si>
@@ -55,21 +56,9 @@
     <t>Aqua</t>
   </si>
   <si>
-    <t>Salutation Type</t>
-  </si>
-  <si>
-    <t>FirstName</t>
-  </si>
-  <si>
     <t>LastName</t>
   </si>
   <si>
-    <t>Mr.</t>
-  </si>
-  <si>
-    <t>Modi</t>
-  </si>
-  <si>
     <t>Gandhi</t>
   </si>
   <si>
@@ -77,12 +66,6 @@
   </si>
   <si>
     <t>India</t>
-  </si>
-  <si>
-    <t>Mrs</t>
-  </si>
-  <si>
-    <t>Sonia</t>
   </si>
 </sst>
 </file>
@@ -498,7 +481,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="B1" sqref="B1:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -556,10 +539,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N15" sqref="N15"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -567,55 +550,55 @@
     <col min="2" max="2" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
         <v>11</v>
       </c>
-      <c r="C1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>13</v>
       </c>
-      <c r="E1" t="s">
-        <v>17</v>
-      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" t="s">
         <v>14</v>
       </c>
-      <c r="C2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" t="s">
-        <v>18</v>
-      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" t="s">
-        <v>20</v>
+      <c r="B3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added one more Test case in both Login and Leads
</commit_message>
<xml_diff>
--- a/src/TestData/Data.xlsx
+++ b/src/TestData/Data.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Leads" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A2:N19"/>
+  <oleSize ref="A1:N18"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="16">
   <si>
     <t>TCName</t>
   </si>
@@ -66,6 +66,9 @@
   </si>
   <si>
     <t>India</t>
+  </si>
+  <si>
+    <t>Modi</t>
   </si>
 </sst>
 </file>
@@ -187,7 +190,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -198,6 +201,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -481,7 +485,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:C3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -542,7 +546,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -589,13 +593,13 @@
         <v>7</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" t="s">
-        <v>12</v>
+        <v>5</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>15</v>
       </c>
       <c r="E3" t="s">
         <v>14</v>

</xml_diff>